<commit_message>
Update Streamlit app and fix dependencies
</commit_message>
<xml_diff>
--- a/waste_log.xlsx
+++ b/waste_log.xlsx
@@ -446,7 +446,11 @@
           <t>2025-03-03</t>
         </is>
       </c>
-      <c r="C1" s="1" t="n"/>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2025-03-05</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="18" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
@@ -458,7 +462,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1">

</xml_diff>